<commit_message>
more update to files
</commit_message>
<xml_diff>
--- a/db/seed_csv/fuel_data.xlsx
+++ b/db/seed_csv/fuel_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="12540" windowWidth="28500" windowHeight="11720" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="12020" windowWidth="28500" windowHeight="5900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -227,12 +227,6 @@
     <t>6.9782 </t>
   </si>
   <si>
-    <t>95_BFP</t>
-  </si>
-  <si>
-    <t>95_Coast</t>
-  </si>
-  <si>
     <t>Exchange_Rate</t>
   </si>
   <si>
@@ -275,12 +269,6 @@
     <t>Petroleum_Products_Levy</t>
   </si>
   <si>
-    <t>2ndary_Distribution</t>
-  </si>
-  <si>
-    <t>2ndary_Storage</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
@@ -291,6 +279,18 @@
   </si>
   <si>
     <t>http://www.energy.gov.za/files/petroleum_frame.html</t>
+  </si>
+  <si>
+    <t>Full_95_Coast</t>
+  </si>
+  <si>
+    <t>Basic_Fuel_Price</t>
+  </si>
+  <si>
+    <t>Secondary_Storage</t>
+  </si>
+  <si>
+    <t>Secondary_Distribution</t>
   </si>
 </sst>
 </file>
@@ -435,8 +435,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -504,11 +510,17 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -788,7 +800,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T2" sqref="T2"/>
+      <selection pane="bottomLeft" activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -819,64 +831,64 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="L1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="L1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
@@ -896,10 +908,10 @@
         <v>17.93</v>
       </c>
       <c r="T2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -919,10 +931,10 @@
         <v>17.79</v>
       </c>
       <c r="T3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -942,10 +954,10 @@
         <v>17.690000000000001</v>
       </c>
       <c r="T4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
@@ -965,10 +977,10 @@
         <v>19.46</v>
       </c>
       <c r="T5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -988,10 +1000,10 @@
         <v>20.78</v>
       </c>
       <c r="T6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
@@ -1011,10 +1023,10 @@
         <v>19.12</v>
       </c>
       <c r="T7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
@@ -1034,10 +1046,10 @@
         <v>18.559999999999999</v>
       </c>
       <c r="T8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
@@ -1057,10 +1069,10 @@
         <v>19.559999999999999</v>
       </c>
       <c r="T9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
@@ -1080,10 +1092,10 @@
         <v>20.190000000000001</v>
       </c>
       <c r="T10" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
@@ -1103,10 +1115,10 @@
         <v>22.14</v>
       </c>
       <c r="T11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
@@ -1126,10 +1138,10 @@
         <v>23.43</v>
       </c>
       <c r="T12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
@@ -1149,10 +1161,10 @@
         <v>22.25</v>
       </c>
       <c r="T13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U13" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
@@ -1172,10 +1184,10 @@
         <v>23.51</v>
       </c>
       <c r="T14" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U14" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
@@ -1195,10 +1207,10 @@
         <v>23.29</v>
       </c>
       <c r="T15" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
@@ -1218,10 +1230,10 @@
         <v>20.54</v>
       </c>
       <c r="T16" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U16" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
@@ -1241,10 +1253,10 @@
         <v>19.420000000000002</v>
       </c>
       <c r="T17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U17" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
@@ -1264,10 +1276,10 @@
         <v>17.98</v>
       </c>
       <c r="T18" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U18" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.2">
@@ -1287,10 +1299,10 @@
         <v>19.47</v>
       </c>
       <c r="T19" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U19" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
@@ -1310,10 +1322,10 @@
         <v>18.02</v>
       </c>
       <c r="T20" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U20" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
@@ -1333,10 +1345,10 @@
         <v>18.45</v>
       </c>
       <c r="T21" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U21" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
@@ -1356,10 +1368,10 @@
         <v>18.79</v>
       </c>
       <c r="T22" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U22" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.2">
@@ -1379,10 +1391,10 @@
         <v>18.73</v>
       </c>
       <c r="T23" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U23" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.2">
@@ -1402,10 +1414,10 @@
         <v>20.12</v>
       </c>
       <c r="T24" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U24" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.2">
@@ -1425,10 +1437,10 @@
         <v>19.16</v>
       </c>
       <c r="T25" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U25" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.2">
@@ -1448,10 +1460,10 @@
         <v>17.239999999999998</v>
       </c>
       <c r="T26" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U26" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.2">
@@ -1471,10 +1483,10 @@
         <v>15.07</v>
       </c>
       <c r="T27" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U27" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.2">
@@ -1494,10 +1506,10 @@
         <v>14.18</v>
       </c>
       <c r="T28" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U28" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.2">
@@ -1517,10 +1529,10 @@
         <v>13.24</v>
       </c>
       <c r="T29" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U29" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.2">
@@ -1540,10 +1552,10 @@
         <v>13.39</v>
       </c>
       <c r="T30" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U30" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.2">
@@ -1563,10 +1575,10 @@
         <v>13.97</v>
       </c>
       <c r="T31" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U31" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.2">
@@ -1586,10 +1598,10 @@
         <v>12.48</v>
       </c>
       <c r="T32" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U32" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.2">
@@ -1609,10 +1621,10 @@
         <v>12.72</v>
       </c>
       <c r="T33" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U33" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.2">
@@ -1632,10 +1644,10 @@
         <v>12.49</v>
       </c>
       <c r="T34" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U34" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.2">
@@ -1655,10 +1667,10 @@
         <v>13.8</v>
       </c>
       <c r="T35" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U35" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.2">
@@ -1678,10 +1690,10 @@
         <v>13.26</v>
       </c>
       <c r="T36" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U36" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.2">
@@ -1701,10 +1713,10 @@
         <v>11.88</v>
       </c>
       <c r="T37" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U37" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.2">
@@ -1724,10 +1736,10 @@
         <v>10.41</v>
       </c>
       <c r="T38" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U38" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.2">
@@ -1747,10 +1759,10 @@
         <v>11.32</v>
       </c>
       <c r="T39" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U39" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.2">
@@ -1770,10 +1782,10 @@
         <v>10.75</v>
       </c>
       <c r="T40" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U40" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.2">
@@ -1793,10 +1805,10 @@
         <v>12.86</v>
       </c>
       <c r="T41" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U41" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.2">
@@ -1816,10 +1828,10 @@
         <v>15.73</v>
       </c>
       <c r="T42" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U42" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.2">
@@ -1839,10 +1851,10 @@
         <v>16.12</v>
       </c>
       <c r="T43" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U43" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.2">
@@ -1862,10 +1874,10 @@
         <v>16.239999999999998</v>
       </c>
       <c r="T44" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U44" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.2">
@@ -1885,10 +1897,10 @@
         <v>18.75</v>
       </c>
       <c r="T45" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U45" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.2">
@@ -1908,10 +1920,10 @@
         <v>20.21</v>
       </c>
       <c r="T46" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U46" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.2">
@@ -1931,10 +1943,10 @@
         <v>22.37</v>
       </c>
       <c r="T47" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U47" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.2">
@@ -1954,10 +1966,10 @@
         <v>22.19</v>
       </c>
       <c r="T48" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U48" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.2">
@@ -1977,10 +1989,10 @@
         <v>24.22</v>
       </c>
       <c r="T49" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U49" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.2">
@@ -2000,10 +2012,10 @@
         <v>25.01</v>
       </c>
       <c r="T50" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U50" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.2">
@@ -2023,10 +2035,10 @@
         <v>25.21</v>
       </c>
       <c r="T51" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U51" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.2">
@@ -2046,10 +2058,10 @@
         <v>27.15</v>
       </c>
       <c r="T52" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U52" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.2">
@@ -2069,10 +2081,10 @@
         <v>27.49</v>
       </c>
       <c r="T53" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U53" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.2">
@@ -2092,10 +2104,10 @@
         <v>23.45</v>
       </c>
       <c r="T54" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U54" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.2">
@@ -2115,10 +2127,10 @@
         <v>27.23</v>
       </c>
       <c r="T55" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U55" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.2">
@@ -2138,10 +2150,10 @@
         <v>29.62</v>
       </c>
       <c r="T56" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U56" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.2">
@@ -2161,10 +2173,10 @@
         <v>28.16</v>
       </c>
       <c r="T57" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U57" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.2">
@@ -2184,10 +2196,10 @@
         <v>29.41</v>
       </c>
       <c r="T58" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U58" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.2">
@@ -2207,10 +2219,10 @@
         <v>32.08</v>
       </c>
       <c r="T59" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U59" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.2">
@@ -2230,10 +2242,10 @@
         <v>31.4</v>
       </c>
       <c r="T60" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U60" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.2">
@@ -2253,10 +2265,10 @@
         <v>32.33</v>
       </c>
       <c r="T61" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U61" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.2">
@@ -2276,10 +2288,10 @@
         <v>25.28</v>
       </c>
       <c r="T62" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U62" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.2">
@@ -2299,10 +2311,10 @@
         <v>25.95</v>
       </c>
       <c r="T63" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U63" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.2">
@@ -2322,10 +2334,10 @@
         <v>27.24</v>
       </c>
       <c r="T64" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U64" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.2">
@@ -2345,10 +2357,10 @@
         <v>25.02</v>
       </c>
       <c r="T65" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U65" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.2">
@@ -2368,10 +2380,10 @@
         <v>25.66</v>
       </c>
       <c r="T66" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U66" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.2">
@@ -2391,10 +2403,10 @@
         <v>27.55</v>
       </c>
       <c r="T67" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U67" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.2">
@@ -2414,10 +2426,10 @@
         <v>26.97</v>
       </c>
       <c r="T68" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U68" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.2">
@@ -2437,10 +2449,10 @@
         <v>24.8</v>
       </c>
       <c r="T69" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U69" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.2">
@@ -2460,10 +2472,10 @@
         <v>25.81</v>
       </c>
       <c r="T70" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U70" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.2">
@@ -2483,10 +2495,10 @@
         <v>25.03</v>
       </c>
       <c r="T71" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U71" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.2">
@@ -2506,10 +2518,10 @@
         <v>20.73</v>
       </c>
       <c r="T72" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U72" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.2">
@@ -2529,10 +2541,10 @@
         <v>18.690000000000001</v>
       </c>
       <c r="T73" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U73" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.2">
@@ -2552,10 +2564,10 @@
         <v>18.52</v>
       </c>
       <c r="T74" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U74" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.2">
@@ -2575,10 +2587,10 @@
         <v>19.149999999999999</v>
       </c>
       <c r="T75" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U75" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.2">
@@ -2598,10 +2610,10 @@
         <v>19.98</v>
       </c>
       <c r="T76" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U76" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.2">
@@ -2621,10 +2633,10 @@
         <v>23.64</v>
       </c>
       <c r="T77" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U77" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.2">
@@ -2644,10 +2656,10 @@
         <v>25.43</v>
       </c>
       <c r="T78" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U78" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.2">
@@ -2667,10 +2679,10 @@
         <v>25.69</v>
       </c>
       <c r="T79" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U79" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.2">
@@ -2690,10 +2702,10 @@
         <v>24.49</v>
       </c>
       <c r="T80" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U80" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.2">
@@ -2713,10 +2725,10 @@
         <v>25.75</v>
       </c>
       <c r="T81" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U81" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.2">
@@ -2736,10 +2748,10 @@
         <v>26.78</v>
       </c>
       <c r="T82" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U82" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.2">
@@ -2759,10 +2771,10 @@
         <v>28.28</v>
       </c>
       <c r="T83" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U83" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.2">
@@ -2782,10 +2794,10 @@
         <v>27.53</v>
       </c>
       <c r="T84" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U84" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.2">
@@ -2805,10 +2817,10 @@
         <v>24.79</v>
       </c>
       <c r="T85" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U85" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.2">
@@ -2828,10 +2840,10 @@
         <v>27.89</v>
       </c>
       <c r="T86" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U86" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.2">
@@ -2851,10 +2863,10 @@
         <v>30.77</v>
       </c>
       <c r="T87" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U87" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.2">
@@ -2874,10 +2886,10 @@
         <v>32.880000000000003</v>
       </c>
       <c r="T88" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U88" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.2">
@@ -2897,10 +2909,10 @@
         <v>30.36</v>
       </c>
       <c r="T89" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U89" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.2">
@@ -2920,10 +2932,10 @@
         <v>25.49</v>
       </c>
       <c r="T90" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U90" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.2">
@@ -2943,10 +2955,10 @@
         <v>26.06</v>
       </c>
       <c r="T91" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U91" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.2">
@@ -2966,10 +2978,10 @@
         <v>27.91</v>
       </c>
       <c r="T92" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U92" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.2">
@@ -2989,10 +3001,10 @@
         <v>28.59</v>
       </c>
       <c r="T93" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U93" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.2">
@@ -3012,10 +3024,10 @@
         <v>29.68</v>
       </c>
       <c r="T94" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U94" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.2">
@@ -3035,10 +3047,10 @@
         <v>26.88</v>
       </c>
       <c r="T95" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U95" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.2">
@@ -3058,10 +3070,10 @@
         <v>29.01</v>
       </c>
       <c r="T96" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U96" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.2">
@@ -3081,10 +3093,10 @@
         <v>29.12</v>
       </c>
       <c r="T97" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U97" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.2">
@@ -3104,10 +3116,10 @@
         <v>29.95</v>
       </c>
       <c r="T98" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U98" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.2">
@@ -3127,10 +3139,10 @@
         <v>31.4</v>
       </c>
       <c r="T99" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U99" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.2">
@@ -3150,10 +3162,10 @@
         <v>31.32</v>
       </c>
       <c r="T100" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U100" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.2">
@@ -3173,10 +3185,10 @@
         <v>33.67</v>
       </c>
       <c r="T101" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U101" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.2">
@@ -3196,10 +3208,10 @@
         <v>33.71</v>
       </c>
       <c r="T102" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U102" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.2">
@@ -3219,10 +3231,10 @@
         <v>37.630000000000003</v>
       </c>
       <c r="T103" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U103" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.2">
@@ -3242,10 +3254,10 @@
         <v>35.54</v>
       </c>
       <c r="T104" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U104" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.2">
@@ -3265,10 +3277,10 @@
         <v>37.93</v>
       </c>
       <c r="T105" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U105" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.2">
@@ -3288,10 +3300,10 @@
         <v>42.08</v>
       </c>
       <c r="T106" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U106" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.2">
@@ -3311,10 +3323,10 @@
         <v>41.65</v>
       </c>
       <c r="T107" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U107" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="108" spans="1:21" x14ac:dyDescent="0.2">
@@ -3334,10 +3346,10 @@
         <v>46.87</v>
       </c>
       <c r="T108" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U108" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="109" spans="1:21" x14ac:dyDescent="0.2">
@@ -3357,10 +3369,10 @@
         <v>42.23</v>
       </c>
       <c r="T109" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U109" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="110" spans="1:21" x14ac:dyDescent="0.2">
@@ -3380,10 +3392,10 @@
         <v>39.090000000000003</v>
       </c>
       <c r="T110" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U110" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.2">
@@ -3403,10 +3415,10 @@
         <v>42.89</v>
       </c>
       <c r="T111" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U111" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="112" spans="1:21" x14ac:dyDescent="0.2">
@@ -3426,10 +3438,10 @@
         <v>44.56</v>
       </c>
       <c r="T112" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U112" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="113" spans="1:21" x14ac:dyDescent="0.2">
@@ -3449,10 +3461,10 @@
         <v>50.93</v>
       </c>
       <c r="T113" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U113" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="114" spans="1:21" x14ac:dyDescent="0.2">
@@ -3472,10 +3484,10 @@
         <v>50.64</v>
       </c>
       <c r="T114" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U114" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="115" spans="1:21" x14ac:dyDescent="0.2">
@@ -3495,10 +3507,10 @@
         <v>47.81</v>
       </c>
       <c r="T115" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U115" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="116" spans="1:21" x14ac:dyDescent="0.2">
@@ -3518,10 +3530,10 @@
         <v>53.89</v>
       </c>
       <c r="T116" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U116" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="117" spans="1:21" x14ac:dyDescent="0.2">
@@ -3541,10 +3553,10 @@
         <v>56.37</v>
       </c>
       <c r="T117" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U117" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="118" spans="1:21" x14ac:dyDescent="0.2">
@@ -3564,10 +3576,10 @@
         <v>61.87</v>
       </c>
       <c r="T118" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U118" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="119" spans="1:21" x14ac:dyDescent="0.2">
@@ -3587,10 +3599,10 @@
         <v>61.65</v>
       </c>
       <c r="T119" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U119" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="120" spans="1:21" x14ac:dyDescent="0.2">
@@ -3610,10 +3622,10 @@
         <v>58.19</v>
       </c>
       <c r="T120" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U120" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="121" spans="1:21" x14ac:dyDescent="0.2">
@@ -3633,10 +3645,10 @@
         <v>54.98</v>
       </c>
       <c r="T121" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U121" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="122" spans="1:21" x14ac:dyDescent="0.2">
@@ -3656,10 +3668,10 @@
         <v>56.47</v>
       </c>
       <c r="T122" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U122" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="123" spans="1:21" x14ac:dyDescent="0.2">
@@ -3679,10 +3691,10 @@
         <v>54.46</v>
       </c>
       <c r="T123" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U123" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="124" spans="1:21" x14ac:dyDescent="0.2">
@@ -3702,10 +3714,10 @@
         <v>55.49</v>
       </c>
       <c r="T124" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U124" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="125" spans="1:21" x14ac:dyDescent="0.2">
@@ -3725,10 +3737,10 @@
         <v>61.08</v>
       </c>
       <c r="T125" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U125" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="126" spans="1:21" x14ac:dyDescent="0.2">
@@ -3748,10 +3760,10 @@
         <v>65.66</v>
       </c>
       <c r="T126" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U126" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="127" spans="1:21" x14ac:dyDescent="0.2">
@@ -3771,10 +3783,10 @@
         <v>68.8</v>
       </c>
       <c r="T127" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U127" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="128" spans="1:21" x14ac:dyDescent="0.2">
@@ -3794,10 +3806,10 @@
         <v>70.11</v>
       </c>
       <c r="T128" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U128" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="129" spans="1:21" x14ac:dyDescent="0.2">
@@ -3817,10 +3829,10 @@
         <v>72.209999999999994</v>
       </c>
       <c r="T129" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U129" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="130" spans="1:21" x14ac:dyDescent="0.2">
@@ -3840,10 +3852,10 @@
         <v>73.7</v>
       </c>
       <c r="T130" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U130" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="131" spans="1:21" x14ac:dyDescent="0.2">
@@ -3863,10 +3875,10 @@
         <v>65.12</v>
       </c>
       <c r="T131" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U131" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="132" spans="1:21" x14ac:dyDescent="0.2">
@@ -3886,10 +3898,10 @@
         <v>59.11</v>
       </c>
       <c r="T132" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U132" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="133" spans="1:21" x14ac:dyDescent="0.2">
@@ -3909,10 +3921,10 @@
         <v>63.03</v>
       </c>
       <c r="T133" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U133" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="134" spans="1:21" x14ac:dyDescent="0.2">
@@ -3932,10 +3944,10 @@
         <v>58.32</v>
       </c>
       <c r="T134" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U134" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="135" spans="1:21" x14ac:dyDescent="0.2">
@@ -3955,10 +3967,10 @@
         <v>58.02</v>
       </c>
       <c r="T135" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U135" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="136" spans="1:21" x14ac:dyDescent="0.2">
@@ -3978,10 +3990,10 @@
         <v>53.12</v>
       </c>
       <c r="T136" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U136" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="137" spans="1:21" x14ac:dyDescent="0.2">
@@ -4001,10 +4013,10 @@
         <v>57.35</v>
       </c>
       <c r="T137" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U137" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="138" spans="1:21" x14ac:dyDescent="0.2">
@@ -4024,10 +4036,10 @@
         <v>62.1</v>
       </c>
       <c r="T138" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U138" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="139" spans="1:21" x14ac:dyDescent="0.2">
@@ -4047,10 +4059,10 @@
         <v>64.13</v>
       </c>
       <c r="T139" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U139" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="140" spans="1:21" x14ac:dyDescent="0.2">
@@ -4070,10 +4082,10 @@
         <v>66.45</v>
       </c>
       <c r="T140" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U140" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="141" spans="1:21" x14ac:dyDescent="0.2">
@@ -4093,10 +4105,10 @@
         <v>63.33</v>
       </c>
       <c r="T141" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U141" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="142" spans="1:21" x14ac:dyDescent="0.2">
@@ -4116,10 +4128,10 @@
         <v>60.48</v>
       </c>
       <c r="T142" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U142" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="143" spans="1:21" x14ac:dyDescent="0.2">
@@ -4139,10 +4151,10 @@
         <v>71.790000000000006</v>
       </c>
       <c r="T143" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U143" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="144" spans="1:21" x14ac:dyDescent="0.2">
@@ -4162,10 +4174,10 @@
         <v>76.432000000000002</v>
       </c>
       <c r="T144" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U144" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="145" spans="1:21" x14ac:dyDescent="0.2">
@@ -4185,10 +4197,10 @@
         <v>82.78</v>
       </c>
       <c r="T145" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U145" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="146" spans="1:21" x14ac:dyDescent="0.2">
@@ -4208,10 +4220,10 @@
         <v>92.91</v>
       </c>
       <c r="T146" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U146" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="147" spans="1:21" x14ac:dyDescent="0.2">
@@ -4231,10 +4243,10 @@
         <v>90.37</v>
       </c>
       <c r="T147" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U147" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="148" spans="1:21" x14ac:dyDescent="0.2">
@@ -4254,10 +4266,10 @@
         <v>92.16</v>
       </c>
       <c r="T148" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U148" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="149" spans="1:21" x14ac:dyDescent="0.2">
@@ -4277,10 +4289,10 @@
         <v>94.74</v>
       </c>
       <c r="T149" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U149" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="150" spans="1:21" x14ac:dyDescent="0.2">
@@ -4300,10 +4312,10 @@
         <v>102.4</v>
       </c>
       <c r="T150" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U150" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="151" spans="1:21" x14ac:dyDescent="0.2">
@@ -4323,10 +4335,10 @@
         <v>108.37</v>
       </c>
       <c r="T151" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U151" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="152" spans="1:21" x14ac:dyDescent="0.2">
@@ -4346,10 +4358,10 @@
         <v>122.25</v>
       </c>
       <c r="T152" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U152" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="153" spans="1:21" x14ac:dyDescent="0.2">
@@ -4369,10 +4381,10 @@
         <v>131.54</v>
       </c>
       <c r="T153" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U153" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="154" spans="1:21" x14ac:dyDescent="0.2">
@@ -4392,10 +4404,10 @@
         <v>133.63999999999999</v>
       </c>
       <c r="T154" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U154" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="155" spans="1:21" x14ac:dyDescent="0.2">
@@ -4415,10 +4427,10 @@
         <v>113</v>
       </c>
       <c r="T155" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U155" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="156" spans="1:21" x14ac:dyDescent="0.2">
@@ -4438,10 +4450,10 @@
         <v>99.08</v>
       </c>
       <c r="T156" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U156" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="157" spans="1:21" x14ac:dyDescent="0.2">
@@ -4461,10 +4473,10 @@
         <v>75.33</v>
       </c>
       <c r="T157" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U157" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="158" spans="1:21" x14ac:dyDescent="0.2">
@@ -4484,10 +4496,10 @@
         <v>53.11</v>
       </c>
       <c r="T158" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U158" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="159" spans="1:21" x14ac:dyDescent="0.2">
@@ -4507,10 +4519,10 @@
         <v>39.988999999999997</v>
       </c>
       <c r="T159" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U159" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="160" spans="1:21" x14ac:dyDescent="0.2">
@@ -4530,10 +4542,10 @@
         <v>43.548000000000002</v>
       </c>
       <c r="T160" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U160" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="161" spans="1:21" x14ac:dyDescent="0.2">
@@ -4553,10 +4565,10 @@
         <v>43.07</v>
       </c>
       <c r="T161" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U161" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="162" spans="1:21" x14ac:dyDescent="0.2">
@@ -4576,10 +4588,10 @@
         <v>46.543999999999997</v>
       </c>
       <c r="T162" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U162" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="163" spans="1:21" x14ac:dyDescent="0.2">
@@ -4599,10 +4611,10 @@
         <v>50.274000000000001</v>
       </c>
       <c r="T163" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U163" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="164" spans="1:21" x14ac:dyDescent="0.2">
@@ -4622,10 +4634,10 @@
         <v>56.576999999999998</v>
       </c>
       <c r="T164" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U164" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="165" spans="1:21" x14ac:dyDescent="0.2">
@@ -4645,10 +4657,10 @@
         <v>68.34</v>
       </c>
       <c r="T165" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U165" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="166" spans="1:21" x14ac:dyDescent="0.2">
@@ -4668,10 +4680,10 @@
         <v>64.89</v>
       </c>
       <c r="T166" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U166" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="167" spans="1:21" x14ac:dyDescent="0.2">
@@ -4691,10 +4703,10 @@
         <v>72.66</v>
       </c>
       <c r="T167" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U167" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="168" spans="1:21" x14ac:dyDescent="0.2">
@@ -4714,10 +4726,10 @@
         <v>67.84</v>
       </c>
       <c r="T168" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U168" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="169" spans="1:21" x14ac:dyDescent="0.2">
@@ -4737,10 +4749,10 @@
         <v>72.92</v>
       </c>
       <c r="T169" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U169" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="170" spans="1:21" x14ac:dyDescent="0.2">
@@ -4760,10 +4772,10 @@
         <v>76.599999999999994</v>
       </c>
       <c r="T170" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U170" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="171" spans="1:21" x14ac:dyDescent="0.2">
@@ -4783,10 +4795,10 @@
         <v>74.31</v>
       </c>
       <c r="T171" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U171" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="172" spans="1:21" x14ac:dyDescent="0.2">
@@ -4806,10 +4818,10 @@
         <v>76.84</v>
       </c>
       <c r="T172" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U172" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="173" spans="1:21" x14ac:dyDescent="0.2">
@@ -4829,10 +4841,10 @@
         <v>73.17</v>
       </c>
       <c r="T173" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U173" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="174" spans="1:21" x14ac:dyDescent="0.2">
@@ -4852,10 +4864,10 @@
         <v>78.89</v>
       </c>
       <c r="T174" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U174" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="175" spans="1:21" x14ac:dyDescent="0.2">
@@ -4875,10 +4887,10 @@
         <v>85.75</v>
       </c>
       <c r="T175" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U175" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="176" spans="1:21" x14ac:dyDescent="0.2">
@@ -4898,10 +4910,10 @@
         <v>76.3</v>
       </c>
       <c r="T176" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U176" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="177" spans="1:21" x14ac:dyDescent="0.2">
@@ -4921,10 +4933,10 @@
         <v>74.61</v>
       </c>
       <c r="T177" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U177" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="178" spans="1:21" x14ac:dyDescent="0.2">
@@ -4944,10 +4956,10 @@
         <v>78.680000000000007</v>
       </c>
       <c r="T178" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U178" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="179" spans="1:21" x14ac:dyDescent="0.2">
@@ -4967,10 +4979,10 @@
         <v>77.39</v>
       </c>
       <c r="T179" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U179" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="180" spans="1:21" x14ac:dyDescent="0.2">
@@ -4990,10 +5002,10 @@
         <v>77.37</v>
       </c>
       <c r="T180" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U180" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="181" spans="1:21" x14ac:dyDescent="0.2">
@@ -5013,10 +5025,10 @@
         <v>82.73</v>
       </c>
       <c r="T181" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U181" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="182" spans="1:21" x14ac:dyDescent="0.2">
@@ -5036,10 +5048,10 @@
         <v>85.15</v>
       </c>
       <c r="T182" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U182" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="183" spans="1:21" x14ac:dyDescent="0.2">
@@ -5059,10 +5071,10 @@
         <v>90.77</v>
       </c>
       <c r="T183" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U183" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="184" spans="1:21" x14ac:dyDescent="0.2">
@@ -5082,10 +5094,10 @@
         <v>95.97</v>
       </c>
       <c r="T184" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U184" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="185" spans="1:21" x14ac:dyDescent="0.2">
@@ -5105,10 +5117,10 @@
         <v>102.37</v>
       </c>
       <c r="T185" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U185" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="186" spans="1:21" x14ac:dyDescent="0.2">
@@ -5128,10 +5140,10 @@
         <v>114.41</v>
       </c>
       <c r="T186" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U186" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="187" spans="1:21" x14ac:dyDescent="0.2">
@@ -5151,10 +5163,10 @@
         <v>123.49</v>
       </c>
       <c r="T187" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U187" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="188" spans="1:21" x14ac:dyDescent="0.2">
@@ -5174,10 +5186,10 @@
         <v>116.15</v>
       </c>
       <c r="T188" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U188" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="189" spans="1:21" x14ac:dyDescent="0.2">
@@ -5197,10 +5209,10 @@
         <v>114.19</v>
       </c>
       <c r="T189" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U189" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="190" spans="1:21" x14ac:dyDescent="0.2">
@@ -5220,10 +5232,10 @@
         <v>116.88</v>
       </c>
       <c r="T190" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U190" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="191" spans="1:21" x14ac:dyDescent="0.2">
@@ -5243,10 +5255,10 @@
         <v>110.67</v>
       </c>
       <c r="T191" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U191" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="192" spans="1:21" x14ac:dyDescent="0.2">
@@ -5266,10 +5278,10 @@
         <v>113.61</v>
       </c>
       <c r="T192" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U192" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="193" spans="1:21" x14ac:dyDescent="0.2">
@@ -5289,10 +5301,10 @@
         <v>109.28</v>
       </c>
       <c r="T193" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U193" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="194" spans="1:21" x14ac:dyDescent="0.2">
@@ -5312,10 +5324,10 @@
         <v>110.51</v>
       </c>
       <c r="T194" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U194" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="195" spans="1:21" x14ac:dyDescent="0.2">
@@ -5335,10 +5347,10 @@
         <v>107.96</v>
       </c>
       <c r="T195" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U195" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="196" spans="1:21" x14ac:dyDescent="0.2">
@@ -5358,10 +5370,10 @@
         <v>110.42</v>
       </c>
       <c r="T196" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U196" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="197" spans="1:21" x14ac:dyDescent="0.2">
@@ -5381,10 +5393,10 @@
         <v>126.39</v>
       </c>
       <c r="T197" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U197" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="198" spans="1:21" x14ac:dyDescent="0.2">
@@ -5404,10 +5416,10 @@
         <v>125.42</v>
       </c>
       <c r="T198" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U198" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="199" spans="1:21" x14ac:dyDescent="0.2">
@@ -5427,10 +5439,10 @@
         <v>120.18</v>
       </c>
       <c r="T199" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U199" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="200" spans="1:21" x14ac:dyDescent="0.2">
@@ -5450,10 +5462,10 @@
         <v>110.27</v>
       </c>
       <c r="T200" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U200" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="201" spans="1:21" x14ac:dyDescent="0.2">
@@ -5473,10 +5485,10 @@
         <v>95.22</v>
       </c>
       <c r="T201" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U201" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="202" spans="1:21" x14ac:dyDescent="0.2">
@@ -5496,10 +5508,10 @@
         <v>102.04</v>
       </c>
       <c r="T202" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U202" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="203" spans="1:21" x14ac:dyDescent="0.2">
@@ -5519,10 +5531,10 @@
         <v>113.51</v>
       </c>
       <c r="T203" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U203" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="204" spans="1:21" x14ac:dyDescent="0.2">
@@ -5542,10 +5554,10 @@
         <v>112.96</v>
       </c>
       <c r="T204" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U204" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="205" spans="1:21" x14ac:dyDescent="0.2">
@@ -5565,10 +5577,10 @@
         <v>109.05</v>
       </c>
       <c r="T205" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U205" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="206" spans="1:21" x14ac:dyDescent="0.2">
@@ -5588,10 +5600,10 @@
         <v>109.04</v>
       </c>
       <c r="T206" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U206" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="207" spans="1:21" x14ac:dyDescent="0.2">
@@ -5611,10 +5623,10 @@
         <v>109.13</v>
       </c>
       <c r="T207" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U207" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="208" spans="1:21" x14ac:dyDescent="0.2">
@@ -5634,10 +5646,10 @@
         <v>112.88</v>
       </c>
       <c r="T208" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U208" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="209" spans="1:21" x14ac:dyDescent="0.2">
@@ -5657,10 +5669,10 @@
         <v>116.28</v>
       </c>
       <c r="T209" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U209" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="210" spans="1:21" x14ac:dyDescent="0.2">
@@ -5680,10 +5692,10 @@
         <v>108.44</v>
       </c>
       <c r="T210" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U210" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="211" spans="1:21" x14ac:dyDescent="0.2">
@@ -5703,10 +5715,10 @@
         <v>102.16</v>
       </c>
       <c r="T211" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U211" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="212" spans="1:21" x14ac:dyDescent="0.2">
@@ -5726,10 +5738,10 @@
         <v>102.62</v>
       </c>
       <c r="T212" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U212" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="213" spans="1:21" x14ac:dyDescent="0.2">
@@ -5749,10 +5761,10 @@
         <v>102.84</v>
       </c>
       <c r="T213" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U213" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="214" spans="1:21" x14ac:dyDescent="0.2">
@@ -5772,10 +5784,10 @@
         <v>108.05</v>
       </c>
       <c r="T214" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U214" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="215" spans="1:21" x14ac:dyDescent="0.2">
@@ -5795,10 +5807,10 @@
         <v>111.07</v>
       </c>
       <c r="T215" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U215" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="216" spans="1:21" x14ac:dyDescent="0.2">
@@ -5818,10 +5830,10 @@
         <v>112.23</v>
       </c>
       <c r="T216" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U216" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="217" spans="1:21" x14ac:dyDescent="0.2">
@@ -5841,10 +5853,10 @@
         <v>109.12</v>
       </c>
       <c r="T217" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U217" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="218" spans="1:21" x14ac:dyDescent="0.2">
@@ -5864,10 +5876,10 @@
         <v>107.82</v>
       </c>
       <c r="T218" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U218" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="219" spans="1:21" x14ac:dyDescent="0.2">
@@ -5887,10 +5899,10 @@
         <v>110.73</v>
       </c>
       <c r="T219" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U219" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="220" spans="1:21" x14ac:dyDescent="0.2">
@@ -5910,10 +5922,10 @@
         <v>108.35</v>
       </c>
       <c r="T220" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U220" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="221" spans="1:21" x14ac:dyDescent="0.2">
@@ -5933,10 +5945,10 @@
         <v>108.87</v>
       </c>
       <c r="T221" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U221" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="222" spans="1:21" x14ac:dyDescent="0.2">
@@ -5956,10 +5968,10 @@
         <v>107.67</v>
       </c>
       <c r="T222" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U222" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="223" spans="1:21" x14ac:dyDescent="0.2">
@@ -5979,10 +5991,10 @@
         <v>108.31</v>
       </c>
       <c r="T223" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U223" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="224" spans="1:21" x14ac:dyDescent="0.2">
@@ -6002,10 +6014,10 @@
         <v>109.69</v>
       </c>
       <c r="T224" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U224" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="225" spans="1:21" x14ac:dyDescent="0.2">
@@ -6025,10 +6037,10 @@
         <v>111.62</v>
       </c>
       <c r="T225" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U225" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="226" spans="1:21" x14ac:dyDescent="0.2">
@@ -6048,10 +6060,10 @@
         <v>106.64</v>
       </c>
       <c r="T226" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U226" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="227" spans="1:21" x14ac:dyDescent="0.2">
@@ -6071,10 +6083,10 @@
         <v>101.57</v>
       </c>
       <c r="T227" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U227" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="228" spans="1:21" x14ac:dyDescent="0.2">
@@ -6094,10 +6106,10 @@
         <v>97.73</v>
       </c>
       <c r="T228" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U228" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="229" spans="1:21" x14ac:dyDescent="0.2">
@@ -6117,10 +6129,10 @@
         <v>87.54</v>
       </c>
       <c r="T229" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U229" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="230" spans="1:21" x14ac:dyDescent="0.2">
@@ -6140,10 +6152,10 @@
         <v>79.75</v>
       </c>
       <c r="T230" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U230" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="231" spans="1:21" x14ac:dyDescent="0.2">
@@ -6163,10 +6175,10 @@
         <v>54.98</v>
       </c>
       <c r="T231" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U231" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="232" spans="1:21" x14ac:dyDescent="0.2">
@@ -6186,10 +6198,10 @@
         <v>48.2</v>
       </c>
       <c r="T232" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U232" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="233" spans="1:21" x14ac:dyDescent="0.2">
@@ -6209,10 +6221,10 @@
         <v>57.93</v>
       </c>
       <c r="T233" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U233" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="234" spans="1:21" x14ac:dyDescent="0.2">
@@ -6232,10 +6244,10 @@
         <v>56.11</v>
       </c>
       <c r="T234" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U234" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="235" spans="1:21" x14ac:dyDescent="0.2">
@@ -6255,10 +6267,10 @@
         <v>59.01</v>
       </c>
       <c r="T235" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U235" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="236" spans="1:21" x14ac:dyDescent="0.2">
@@ -6278,10 +6290,10 @@
         <v>64.36</v>
       </c>
       <c r="T236" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U236" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="237" spans="1:21" x14ac:dyDescent="0.2">
@@ -6301,10 +6313,10 @@
         <v>61.94</v>
       </c>
       <c r="T237" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U237" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="238" spans="1:21" x14ac:dyDescent="0.2">
@@ -6324,10 +6336,10 @@
         <v>56.72</v>
       </c>
       <c r="T238" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U238" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="239" spans="1:21" x14ac:dyDescent="0.2">
@@ -6347,10 +6359,10 @@
         <v>46.56</v>
       </c>
       <c r="T239" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U239" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="240" spans="1:21" x14ac:dyDescent="0.2">
@@ -6370,10 +6382,10 @@
         <v>47.79</v>
       </c>
       <c r="T240" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U240" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="241" spans="1:21" x14ac:dyDescent="0.2">
@@ -6393,10 +6405,10 @@
         <v>48.58</v>
       </c>
       <c r="T241" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U241" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="242" spans="1:21" x14ac:dyDescent="0.2">
@@ -6416,10 +6428,10 @@
         <v>44.33</v>
       </c>
       <c r="T242" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U242" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="243" spans="1:21" x14ac:dyDescent="0.2">
@@ -6481,10 +6493,10 @@
         <v>10</v>
       </c>
       <c r="T243" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U243" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="244" spans="1:21" x14ac:dyDescent="0.2">
@@ -6546,10 +6558,10 @@
         <v>10</v>
       </c>
       <c r="T244" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U244" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="245" spans="1:21" x14ac:dyDescent="0.2">
@@ -6611,10 +6623,10 @@
         <v>10</v>
       </c>
       <c r="T245" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U245" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="246" spans="1:21" x14ac:dyDescent="0.2">
@@ -6676,10 +6688,10 @@
         <v>10</v>
       </c>
       <c r="T246" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U246" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="247" spans="1:21" x14ac:dyDescent="0.2">
@@ -6741,10 +6753,10 @@
         <v>10</v>
       </c>
       <c r="T247" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U247" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="248" spans="1:21" x14ac:dyDescent="0.2">
@@ -6806,10 +6818,10 @@
         <v>10</v>
       </c>
       <c r="T248" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U248" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="249" spans="1:21" x14ac:dyDescent="0.2">
@@ -6871,10 +6883,10 @@
         <v>10</v>
       </c>
       <c r="T249" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U249" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="250" spans="1:21" x14ac:dyDescent="0.2">
@@ -6936,10 +6948,10 @@
         <v>10</v>
       </c>
       <c r="T250" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U250" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="251" spans="1:21" x14ac:dyDescent="0.2">
@@ -7001,10 +7013,10 @@
         <v>10</v>
       </c>
       <c r="T251" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U251" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="252" spans="1:21" x14ac:dyDescent="0.2">
@@ -7066,10 +7078,10 @@
         <v>10</v>
       </c>
       <c r="T252" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U252" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="253" spans="1:21" x14ac:dyDescent="0.2">
@@ -7131,10 +7143,10 @@
         <v>10</v>
       </c>
       <c r="T253" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U253" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="254" spans="1:21" x14ac:dyDescent="0.2">
@@ -7196,10 +7208,10 @@
         <v>10</v>
       </c>
       <c r="T254" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U254" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="255" spans="1:21" x14ac:dyDescent="0.2">
@@ -7261,10 +7273,10 @@
         <v>10</v>
       </c>
       <c r="T255" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="U255" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="256" spans="1:21" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
swap out pg on dev for sqlite
</commit_message>
<xml_diff>
--- a/db/seed_csv/fuel_data.xlsx
+++ b/db/seed_csv/fuel_data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -118,7 +118,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="167" formatCode="[$-409]mmm\-yy;@"/>
+    <numFmt numFmtId="166" formatCode="[$-409]mmm\-yy;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -344,16 +344,16 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5210,11 +5210,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="684434768"/>
-        <c:axId val="213738528"/>
+        <c:axId val="-1920159232"/>
+        <c:axId val="-1920155488"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="684434768"/>
+        <c:axId val="-1920159232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5313,14 +5313,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="213738528"/>
+        <c:crossAx val="-1920155488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="213738528"/>
+        <c:axId val="-1920155488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1450.0"/>
@@ -5428,7 +5428,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="684434768"/>
+        <c:crossAx val="-1920159232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6347,9 +6347,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U259"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A217" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H226" sqref="H226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12828,6 +12828,62 @@
         <v>17</v>
       </c>
     </row>
+    <row r="256" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A256" s="17">
+        <v>42767</v>
+      </c>
+      <c r="C256">
+        <v>620.87</v>
+      </c>
+      <c r="F256">
+        <v>620.87</v>
+      </c>
+      <c r="G256">
+        <v>285</v>
+      </c>
+      <c r="H256">
+        <v>4</v>
+      </c>
+      <c r="I256">
+        <v>0</v>
+      </c>
+      <c r="J256">
+        <v>154</v>
+      </c>
+      <c r="K256">
+        <v>41</v>
+      </c>
+      <c r="L256">
+        <v>0.33</v>
+      </c>
+      <c r="M256">
+        <v>35.6</v>
+      </c>
+      <c r="N256">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="O256">
+        <v>17.3</v>
+      </c>
+      <c r="P256">
+        <v>176.4</v>
+      </c>
+      <c r="Q256">
+        <v>0</v>
+      </c>
+      <c r="R256">
+        <v>0</v>
+      </c>
+      <c r="S256">
+        <v>10</v>
+      </c>
+      <c r="T256" t="s">
+        <v>18</v>
+      </c>
+      <c r="U256" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A257" s="20"/>
     </row>
@@ -12844,8 +12900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
get data update model
</commit_message>
<xml_diff>
--- a/db/seed_csv/fuel_data.xlsx
+++ b/db/seed_csv/fuel_data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="-17720" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="9180" windowWidth="28800" windowHeight="8740" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -422,6 +422,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5213,11 +5214,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="40262304"/>
-        <c:axId val="14811936"/>
+        <c:axId val="1388845440"/>
+        <c:axId val="1488984832"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="40262304"/>
+        <c:axId val="1388845440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5249,6 +5250,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5315,14 +5317,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14811936"/>
+        <c:crossAx val="1488984832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="14811936"/>
+        <c:axId val="1488984832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1450.0"/>
@@ -5370,6 +5372,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5429,7 +5432,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40262304"/>
+        <c:crossAx val="1388845440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5443,6 +5446,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6345,11 +6349,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U259"/>
+  <dimension ref="A1:U264"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A259" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B259" sqref="B259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14024,6 +14028,331 @@
         <v>17</v>
       </c>
     </row>
+    <row r="260" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A260" s="16">
+        <v>42887</v>
+      </c>
+      <c r="B260" s="1">
+        <v>1305</v>
+      </c>
+      <c r="C260">
+        <v>572.66999999999996</v>
+      </c>
+      <c r="D260">
+        <v>13.258699999999999</v>
+      </c>
+      <c r="E260">
+        <v>50.06</v>
+      </c>
+      <c r="F260">
+        <v>572.66999999999996</v>
+      </c>
+      <c r="G260">
+        <v>315</v>
+      </c>
+      <c r="H260">
+        <v>4</v>
+      </c>
+      <c r="I260">
+        <v>0</v>
+      </c>
+      <c r="J260">
+        <v>163</v>
+      </c>
+      <c r="K260">
+        <v>41.5</v>
+      </c>
+      <c r="L260">
+        <v>0.33</v>
+      </c>
+      <c r="M260">
+        <v>35.6</v>
+      </c>
+      <c r="N260">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="O260">
+        <v>17.3</v>
+      </c>
+      <c r="P260">
+        <v>176.4</v>
+      </c>
+      <c r="Q260">
+        <v>0</v>
+      </c>
+      <c r="R260">
+        <v>0</v>
+      </c>
+      <c r="S260">
+        <v>10</v>
+      </c>
+      <c r="T260" t="s">
+        <v>18</v>
+      </c>
+      <c r="U260" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="261" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A261" s="16">
+        <v>42917</v>
+      </c>
+      <c r="B261" s="1">
+        <v>1237</v>
+      </c>
+      <c r="C261">
+        <v>504.67</v>
+      </c>
+      <c r="D261">
+        <v>12.8756</v>
+      </c>
+      <c r="E261" s="2">
+        <v>46.48</v>
+      </c>
+      <c r="F261">
+        <v>504.67</v>
+      </c>
+      <c r="G261">
+        <v>315</v>
+      </c>
+      <c r="H261">
+        <v>4</v>
+      </c>
+      <c r="I261">
+        <v>0</v>
+      </c>
+      <c r="J261">
+        <v>163</v>
+      </c>
+      <c r="K261">
+        <v>41.5</v>
+      </c>
+      <c r="L261">
+        <v>0.33</v>
+      </c>
+      <c r="M261">
+        <v>35.6</v>
+      </c>
+      <c r="N261">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="O261">
+        <v>17.3</v>
+      </c>
+      <c r="P261">
+        <v>176.4</v>
+      </c>
+      <c r="Q261">
+        <v>0</v>
+      </c>
+      <c r="R261">
+        <v>0</v>
+      </c>
+      <c r="S261">
+        <v>10</v>
+      </c>
+      <c r="T261" t="s">
+        <v>18</v>
+      </c>
+      <c r="U261" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="262" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A262" s="16">
+        <v>42948</v>
+      </c>
+      <c r="B262" s="1">
+        <v>1256</v>
+      </c>
+      <c r="C262">
+        <v>523.66999999999996</v>
+      </c>
+      <c r="D262">
+        <v>13.15</v>
+      </c>
+      <c r="E262" s="2">
+        <v>48.23</v>
+      </c>
+      <c r="F262">
+        <v>523.66999999999996</v>
+      </c>
+      <c r="G262">
+        <v>315</v>
+      </c>
+      <c r="H262">
+        <v>4</v>
+      </c>
+      <c r="I262">
+        <v>0</v>
+      </c>
+      <c r="J262">
+        <v>163</v>
+      </c>
+      <c r="K262">
+        <v>41.5</v>
+      </c>
+      <c r="L262">
+        <v>0.33</v>
+      </c>
+      <c r="M262">
+        <v>35.6</v>
+      </c>
+      <c r="N262">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="O262">
+        <v>17.3</v>
+      </c>
+      <c r="P262">
+        <v>176.4</v>
+      </c>
+      <c r="Q262">
+        <v>0</v>
+      </c>
+      <c r="R262">
+        <v>0</v>
+      </c>
+      <c r="S262">
+        <v>10</v>
+      </c>
+      <c r="T262" t="s">
+        <v>18</v>
+      </c>
+      <c r="U262" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="263" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A263" s="16">
+        <v>42979</v>
+      </c>
+      <c r="B263" s="1">
+        <v>1323</v>
+      </c>
+      <c r="C263">
+        <v>586.07000000000005</v>
+      </c>
+      <c r="D263" s="2">
+        <v>13.215199999999999</v>
+      </c>
+      <c r="E263" s="2">
+        <v>51.66</v>
+      </c>
+      <c r="F263">
+        <v>586.07000000000005</v>
+      </c>
+      <c r="G263">
+        <v>315</v>
+      </c>
+      <c r="H263">
+        <v>4</v>
+      </c>
+      <c r="I263">
+        <v>0</v>
+      </c>
+      <c r="J263">
+        <v>163</v>
+      </c>
+      <c r="K263">
+        <v>41.5</v>
+      </c>
+      <c r="L263">
+        <v>0.33</v>
+      </c>
+      <c r="M263">
+        <v>35.6</v>
+      </c>
+      <c r="N263">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="O263">
+        <v>17.3</v>
+      </c>
+      <c r="P263">
+        <v>181</v>
+      </c>
+      <c r="Q263">
+        <v>0</v>
+      </c>
+      <c r="R263">
+        <v>0</v>
+      </c>
+      <c r="S263">
+        <v>10</v>
+      </c>
+      <c r="T263" t="s">
+        <v>18</v>
+      </c>
+      <c r="U263" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="264" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A264" s="16">
+        <v>43009</v>
+      </c>
+      <c r="B264" s="1">
+        <v>1352</v>
+      </c>
+      <c r="C264">
+        <v>615.07000000000005</v>
+      </c>
+      <c r="D264">
+        <v>13.1317</v>
+      </c>
+      <c r="E264" s="2">
+        <v>55.99</v>
+      </c>
+      <c r="F264">
+        <v>615.07000000000005</v>
+      </c>
+      <c r="G264">
+        <v>315</v>
+      </c>
+      <c r="H264">
+        <v>4</v>
+      </c>
+      <c r="I264">
+        <v>0</v>
+      </c>
+      <c r="J264">
+        <v>163</v>
+      </c>
+      <c r="K264">
+        <v>41.5</v>
+      </c>
+      <c r="L264">
+        <v>0.33</v>
+      </c>
+      <c r="M264">
+        <v>35.6</v>
+      </c>
+      <c r="N264">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="O264">
+        <v>17.3</v>
+      </c>
+      <c r="P264">
+        <v>181</v>
+      </c>
+      <c r="Q264">
+        <v>0</v>
+      </c>
+      <c r="R264">
+        <v>0</v>
+      </c>
+      <c r="S264">
+        <v>10</v>
+      </c>
+      <c r="T264" t="s">
+        <v>18</v>
+      </c>
+      <c r="U264" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -14034,7 +14363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J259"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
       <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>

</xml_diff>